<commit_message>
updated thesis and arpa errors difference
</commit_message>
<xml_diff>
--- a/thesis_graphs.xlsx
+++ b/thesis_graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1F81D2-3775-4A7C-B325-A7BA3B500655}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981301EB-1A2D-4894-9861-2E5B3391B3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="3675" windowWidth="21555" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>sm1</t>
   </si>
@@ -99,6 +99,60 @@
   </si>
   <si>
     <t>011_0074</t>
+  </si>
+  <si>
+    <t>model_transcription</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>111_0627</t>
+  </si>
+  <si>
+    <t>expect</t>
+  </si>
+  <si>
+    <t>roger what is your position</t>
+  </si>
+  <si>
+    <t>101_0199</t>
+  </si>
+  <si>
+    <t>roger ah what is your position</t>
+  </si>
+  <si>
+    <t>golf bravo victor juliett india is identified good afternoon</t>
+  </si>
+  <si>
+    <t>051_0227</t>
+  </si>
+  <si>
+    <t>goll bravo victor juliett india is identified good afternoon</t>
+  </si>
+  <si>
+    <t>{'golf'}</t>
+  </si>
+  <si>
+    <t>{'exact'}</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>set()</t>
+  </si>
+  <si>
+    <t>japan air four one nine contact milan one three four five two bye</t>
+  </si>
+  <si>
+    <t>101_0308</t>
+  </si>
+  <si>
+    <t>german air four one nine contact milan one three four five two bye</t>
+  </si>
+  <si>
+    <t>{'japan'}</t>
   </si>
 </sst>
 </file>
@@ -182,6 +236,24 @@
     <tableColumn id="10" xr3:uid="{CFD13D0B-EE37-4953-AE4C-808BF00551A3}" name="length_sec"/>
     <tableColumn id="11" xr3:uid="{986630E7-5BC0-42ED-81EE-59192B30A25B}" name="recording_id"/>
     <tableColumn id="12" xr3:uid="{7314666C-096A-449B-83B2-DBC06FDB401F}" name="recording_startpos_sec" totalsRowFunction="sum"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7C0375B-24BF-40AA-86F0-196B8E63FDC1}" name="Table2" displayName="Table2" ref="A9:D13" totalsRowShown="0">
+  <autoFilter ref="A9:D13" xr:uid="{93D5DBEE-53D1-48B8-B33C-CE3B0FAAA96A}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C0F6FE52-771F-45D6-BDD8-8B9226D6967F}" name="transcription"/>
+    <tableColumn id="2" xr3:uid="{5F67B1BD-0EF4-41AC-B4D7-0D5588429542}" name="recording_id"/>
+    <tableColumn id="3" xr3:uid="{5A59900E-7471-40D5-8C86-239D6F21FA22}" name="model_transcription"/>
+    <tableColumn id="4" xr3:uid="{288FFD74-A31D-483F-A689-1BCC933BA221}" name="difference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,17 +522,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L5"/>
+  <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L5"/>
+      <selection activeCell="A9" sqref="A9:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
@@ -615,10 +687,82 @@
         <v>2210.622625</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>